<commit_message>
Graphs created and data processor updated
</commit_message>
<xml_diff>
--- a/CMS/Post_Site_Total_Alarms.xlsx
+++ b/CMS/Post_Site_Total_Alarms.xlsx
@@ -434,6 +434,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>ARN</t>
@@ -441,53 +446,53 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>PKV</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>STL</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>THL</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>AZC</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>PKV</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>SDU</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>STL</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>THL</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>_20240226</t>
+          <t>20240226</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>69</v>
       </c>
       <c r="C2" t="n">
+        <v>159</v>
+      </c>
+      <c r="D2" t="n">
+        <v>68</v>
+      </c>
+      <c r="E2" t="n">
+        <v>110</v>
+      </c>
+      <c r="F2" t="n">
         <v>220</v>
       </c>
-      <c r="D2" t="n">
-        <v>159</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="G2" t="n">
         <v>39</v>
-      </c>
-      <c r="F2" t="n">
-        <v>68</v>
-      </c>
-      <c r="G2" t="n">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20240304 and 20240305 updates
</commit_message>
<xml_diff>
--- a/CMS/Post_Site_Total_Alarms.xlsx
+++ b/CMS/Post_Site_Total_Alarms.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,6 +595,56 @@
         <v>67</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>20240304</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>72</v>
+      </c>
+      <c r="C7" t="n">
+        <v>156</v>
+      </c>
+      <c r="D7" t="n">
+        <v>69</v>
+      </c>
+      <c r="E7" t="n">
+        <v>107</v>
+      </c>
+      <c r="F7" t="n">
+        <v>162</v>
+      </c>
+      <c r="G7" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>20240305</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>71</v>
+      </c>
+      <c r="C8" t="n">
+        <v>339</v>
+      </c>
+      <c r="D8" t="n">
+        <v>68</v>
+      </c>
+      <c r="E8" t="n">
+        <v>107</v>
+      </c>
+      <c r="F8" t="n">
+        <v>167</v>
+      </c>
+      <c r="G8" t="n">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>